<commit_message>
Updates to unit tests per refactoring made in TestHelper class so that unit tests per complete file can be ran at a time. Added PR 3878 suggestion as well.
</commit_message>
<xml_diff>
--- a/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/TestUtils/Files/TestCommittedProjects.xlsx
+++ b/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/TestUtils/Files/TestCommittedProjects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\iAM\BridgeCareApp\AppliedResearchAssociates.iAM.UnitTestsCore\TestData\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aborgaonkar\source\repos\Infrastructure Asset Management\BridgeCareApp\AppliedResearchAssociates.iAM.UnitTestsCore\TestUtils\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EECBE7-40DA-48E2-BC9D-1B273A0B8939}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B630F85-0782-4EAC-AA68-04CF996E0C3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Committed Projects" sheetId="1" r:id="rId1"/>
@@ -444,7 +444,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -529,7 +529,7 @@
         <v>17</v>
       </c>
       <c r="D2">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="E2">
         <v>1</v>

</xml_diff>

<commit_message>
First draft committed project test data
</commit_message>
<xml_diff>
--- a/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/TestUtils/Files/TestCommittedProjects.xlsx
+++ b/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/TestUtils/Files/TestCommittedProjects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aborgaonkar\source\repos\Infrastructure Asset Management\BridgeCareApp\AppliedResearchAssociates.iAM.UnitTestsCore\TestUtils\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Source\Repos\Infrastructure Asset Management\BridgeCareApp\AppliedResearchAssociates.iAM.UnitTestsCore\TestUtils\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B630F85-0782-4EAC-AA68-04CF996E0C3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC89CCBF-A8B4-465B-ADBC-1A8FFE69D844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Committed Projects" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>Test Name</t>
+    <t>Interstate</t>
   </si>
 </sst>
 </file>
@@ -444,7 +444,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>